<commit_message>
Fixed concurrent req check
</commit_message>
<xml_diff>
--- a/inputs/prompts.xlsx
+++ b/inputs/prompts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -415,9 +415,6 @@
       <c r="D1" t="str">
         <v>video_id</v>
       </c>
-      <c r="E1" t="str">
-        <v>ref_img</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -430,7 +427,7 @@
         <v>success</v>
       </c>
       <c r="D2" t="str">
-        <v>task_01k2nyc7aze6wa88ee681mg6qj</v>
+        <v>task_01k2sd81t6fnja114fgn43mydt</v>
       </c>
     </row>
     <row r="3">
@@ -444,13 +441,12 @@
         <v>success</v>
       </c>
       <c r="D3" t="str">
-        <v>task_01k2nyckkgfvj8wgzhxaeseqht</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Make this girl animate, wind is blowing gently from left to right. Keep the camrea steady
-</v>
+        <v>task_01k2sda8fdfgg9hx4948a3p9st</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>aerial shot of Victoria Waterfal, Zimbabwe</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -459,15 +455,40 @@
         <v>success</v>
       </c>
       <c r="D4" t="str">
-        <v>task_01k2nyy8y5eqeagzkyyaz1xyv8</v>
-      </c>
-      <c r="E4" t="str">
-        <v>girl.webp</v>
+        <v>task_01k2sdc5mpfk7rtgt397bq0ecy</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>aerial video of Lumangwe waterfal</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>success</v>
+      </c>
+      <c r="D5" t="str">
+        <v>task_01k2sddqq2e42rs2cefmypkryq</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>aerial video of Singapore Marinabay</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>success</v>
+      </c>
+      <c r="D6" t="str">
+        <v>task_01k2sdfqjbfe8szhjdqmba5xvq</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>